<commit_message>
minor change in table2
</commit_message>
<xml_diff>
--- a/results/table2/MV.xlsx
+++ b/results/table2/MV.xlsx
@@ -467,7 +467,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D46"/>
+  <dimension ref="A1:D44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -939,17 +939,17 @@
       </c>
       <c r="B25" s="1" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>0</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>1362 (90.6)</t>
+          <t>1379 (91.7)</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>6634 (93.8)</t>
+          <t>6680 (94.4)</t>
         </is>
       </c>
     </row>
@@ -957,35 +957,39 @@
       <c r="A26" s="1" t="n"/>
       <c r="B26" s="1" t="inlineStr">
         <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>124 (8.3)</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>393 (5.6)</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="inlineStr">
+        <is>
+          <t>Diabetes Type, n (%)</t>
+        </is>
+      </c>
+      <c r="B27" s="1" t="inlineStr">
+        <is>
           <t>1.0</t>
         </is>
       </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>3 (0.2)</t>
-        </is>
-      </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>1 (0.0)</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" s="1" t="n"/>
-      <c r="B27" s="1" t="inlineStr">
-        <is>
-          <t>2.0</t>
-        </is>
-      </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>14 (0.9)</t>
+          <t>33 (2.2)</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>45 (0.6)</t>
+          <t>167 (2.4)</t>
         </is>
       </c>
     </row>
@@ -993,82 +997,86 @@
       <c r="A28" s="1" t="n"/>
       <c r="B28" s="1" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>2.0</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>124 (8.3)</t>
+          <t>582 (38.7)</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>393 (5.6)</t>
+          <t>1988 (28.1)</t>
         </is>
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="1" t="inlineStr">
-        <is>
-          <t>Diabetes Type, n (%)</t>
-        </is>
-      </c>
+      <c r="A29" s="1" t="n"/>
       <c r="B29" s="1" t="inlineStr">
         <is>
+          <t>Absent</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>888 (59.1)</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>4918 (69.5)</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="inlineStr">
+        <is>
+          <t>Connective Tissue Disease, n (%)</t>
+        </is>
+      </c>
+      <c r="B30" s="1" t="inlineStr">
+        <is>
           <t>1.0</t>
         </is>
       </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>33 (2.2)</t>
-        </is>
-      </c>
-      <c r="D29" t="inlineStr">
-        <is>
-          <t>167 (2.4)</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" s="1" t="n"/>
-      <c r="B30" s="1" t="inlineStr">
-        <is>
-          <t>2.0</t>
-        </is>
-      </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>582 (38.7)</t>
+          <t>62 (4.1)</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>1988 (28.1)</t>
+          <t>305 (4.3)</t>
         </is>
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="1" t="n"/>
+      <c r="A31" s="1" t="inlineStr">
+        <is>
+          <t>Pneumonia, n (%)</t>
+        </is>
+      </c>
       <c r="B31" s="1" t="inlineStr">
         <is>
-          <t>Absent</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>888 (59.1)</t>
+          <t>103 (6.9)</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>4918 (69.5)</t>
+          <t>384 (5.4)</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="inlineStr">
         <is>
-          <t>Connective Tissue Disease, n (%)</t>
+          <t>Urinary Tract Infection, n (%)</t>
         </is>
       </c>
       <c r="B32" s="1" t="inlineStr">
@@ -1078,19 +1086,19 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>62 (4.1)</t>
+          <t>4 (0.3)</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>305 (4.3)</t>
+          <t>33 (0.5)</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="inlineStr">
         <is>
-          <t>Pneumonia, n (%)</t>
+          <t>Biliary Tract Infection, n (%)</t>
         </is>
       </c>
       <c r="B33" s="1" t="inlineStr">
@@ -1100,19 +1108,19 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>103 (6.9)</t>
+          <t>1 (0.1)</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>384 (5.4)</t>
+          <t>14 (0.2)</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="inlineStr">
         <is>
-          <t>Urinary Tract Infection, n (%)</t>
+          <t>Skin Infection, n (%)</t>
         </is>
       </c>
       <c r="B34" s="1" t="inlineStr">
@@ -1122,234 +1130,190 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>4 (0.3)</t>
+          <t>2 (0.1)</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>33 (0.5)</t>
+          <t>9 (0.1)</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="inlineStr">
         <is>
-          <t>Biliary Tract Infection, n (%)</t>
-        </is>
-      </c>
-      <c r="B35" s="1" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
+          <t>Age, median [Q1,Q3]</t>
+        </is>
+      </c>
+      <c r="B35" s="1" t="inlineStr"/>
       <c r="C35" t="inlineStr">
         <is>
-          <t>1 (0.1)</t>
+          <t>64 [51,76]</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>14 (0.2)</t>
+          <t>68 [58,79]</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="inlineStr">
         <is>
-          <t>Skin Infection, n (%)</t>
-        </is>
-      </c>
-      <c r="B36" s="1" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
+          <t>ICU LOS (days, if deceased), median [Q1,Q3]</t>
+        </is>
+      </c>
+      <c r="B36" s="1" t="inlineStr"/>
       <c r="C36" t="inlineStr">
         <is>
-          <t>2 (0.1)</t>
+          <t>5.83 [3.54,10.17]</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>9 (0.1)</t>
+          <t>5.90 [3.57,10.51]</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="inlineStr">
         <is>
-          <t>Age, median [Q1,Q3]</t>
+          <t>ICU LOS (days, if survived), median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B37" s="1" t="inlineStr"/>
       <c r="C37" t="inlineStr">
         <is>
-          <t>64 [51,76]</t>
+          <t>4.54 [2.96,8.79]</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>68 [58,79]</t>
+          <t>4.42 [2.92,8.17]</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="inlineStr">
         <is>
-          <t>ICU LOS (days, if deceased), median [Q1,Q3]</t>
+          <t>Charlson Comorbidity Index, median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B38" s="1" t="inlineStr"/>
       <c r="C38" t="inlineStr">
         <is>
-          <t>5.83 [3.54,10.17]</t>
+          <t>6 [4,8]</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>5.90 [3.57,10.51]</t>
+          <t>6 [4,8]</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="inlineStr">
         <is>
-          <t>ICU LOS (days, if survived), median [Q1,Q3]</t>
+          <t>SOFA Score (admission), median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B39" s="1" t="inlineStr"/>
       <c r="C39" t="inlineStr">
         <is>
-          <t>4.54 [2.96,8.79]</t>
+          <t>6 [4,9]</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>4.42 [2.92,8.17]</t>
+          <t>6 [4,9]</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="inlineStr">
         <is>
-          <t>Charlson Comorbidity Index, median [Q1,Q3]</t>
+          <t>MV Time (duration in the stay, % of ICU LOS), median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B40" s="1" t="inlineStr"/>
       <c r="C40" t="inlineStr">
         <is>
-          <t>6 [4,8]</t>
+          <t>0.33 [0.16,0.54]</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>6 [4,8]</t>
+          <t>0.29 [0.15,0.48]</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="inlineStr">
         <is>
-          <t>SOFA Score (admission), median [Q1,Q3]</t>
+          <t>MV_init_offset_abs_hours, median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B41" s="1" t="inlineStr"/>
       <c r="C41" t="inlineStr">
         <is>
-          <t>6 [4,9]</t>
+          <t>2.0 [1.0,7.0]</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>6 [4,9]</t>
+          <t>3.0 [1.0,8.0]</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="inlineStr">
         <is>
-          <t>MV Time (duration in the stay, % of ICU LOS), median [Q1,Q3]</t>
+          <t>RRT_init_offset_abs_hours, median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B42" s="1" t="inlineStr"/>
       <c r="C42" t="inlineStr">
         <is>
-          <t>0.33 [0.16,0.54]</t>
+          <t>41.0 [10.0,91.0]</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>0.29 [0.15,0.48]</t>
+          <t>45.0 [12.0,100.2]</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="inlineStr">
         <is>
-          <t>MV_init_offset_abs_hours, median [Q1,Q3]</t>
+          <t>VP_init_offset_abs_hours, median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B43" s="1" t="inlineStr"/>
       <c r="C43" t="inlineStr">
         <is>
-          <t>2.0 [1.0,7.0]</t>
+          <t>3.0 [1.0,11.0]</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>3.0 [1.0,8.0]</t>
+          <t>3.0 [1.0,10.0]</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="inlineStr">
         <is>
-          <t>RRT_init_offset_abs_hours, median [Q1,Q3]</t>
+          <t>Vasopressor Time (duration in the stay, % of ICU LOS), median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B44" s="1" t="inlineStr"/>
       <c r="C44" t="inlineStr">
         <is>
-          <t>41.0 [10.0,91.0]</t>
+          <t>0.25 [0.10,0.48]</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
-        <is>
-          <t>45.0 [12.0,100.2]</t>
-        </is>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" s="1" t="inlineStr">
-        <is>
-          <t>VP_init_offset_abs_hours, median [Q1,Q3]</t>
-        </is>
-      </c>
-      <c r="B45" s="1" t="inlineStr"/>
-      <c r="C45" t="inlineStr">
-        <is>
-          <t>3.0 [1.0,11.0]</t>
-        </is>
-      </c>
-      <c r="D45" t="inlineStr">
-        <is>
-          <t>3.0 [1.0,10.0]</t>
-        </is>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" s="1" t="inlineStr">
-        <is>
-          <t>Vasopressor Time (duration in the stay, % of ICU LOS), median [Q1,Q3]</t>
-        </is>
-      </c>
-      <c r="B46" s="1" t="inlineStr"/>
-      <c r="C46" t="inlineStr">
-        <is>
-          <t>0.25 [0.10,0.48]</t>
-        </is>
-      </c>
-      <c r="D46" t="inlineStr">
         <is>
           <t>0.25 [0.09,0.47]</t>
         </is>
@@ -1358,10 +1322,10 @@
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="C1:D1"/>
+    <mergeCell ref="A25:A26"/>
     <mergeCell ref="A10:A12"/>
-    <mergeCell ref="A29:A31"/>
     <mergeCell ref="A5:A8"/>
-    <mergeCell ref="A25:A28"/>
+    <mergeCell ref="A27:A29"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>